<commit_message>
updated files with predictions (in csv files) and functions. Prediction.py is the function to run. The classifier functions are copied and pasted into here, so those are not needed.
</commit_message>
<xml_diff>
--- a/Chi2_values.xlsx
+++ b/Chi2_values.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethplackowski/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethplackowski/Documents/ML_class/ML_class/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{351D2434-DAF9-464C-982B-8EB404EB8B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE855B-4A9F-CF40-ABA6-670F1C796DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="500" windowWidth="27240" windowHeight="15360" xr2:uid="{C8D6B880-5D87-CA4C-8D1A-AB641C3D46FF}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="15360" xr2:uid="{C8D6B880-5D87-CA4C-8D1A-AB641C3D46FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -388,1830 +388,2389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE96B71-F44A-6644-B295-6C8FCE0229B1}">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <f>_xlfn.CHISQ.INV(1-$B$1,A2)</f>
-        <v>2.7055434540954142</v>
+        <v>6.6348966010212118</v>
       </c>
       <c r="C2">
         <f>_xlfn.CHISQ.INV(1-$C$1,A2)</f>
         <v>3.8414588206941236</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>_xlfn.CHISQ.INV(1-$D$1,A2)</f>
+        <v>7.8794385766224124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" si="0">_xlfn.CHISQ.INV(1-$B$1,A3)</f>
-        <v>4.6051701859880918</v>
+        <v>9.2103403719761818</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="1">_xlfn.CHISQ.INV(1-$C$1,A3)</f>
         <v>5.9914645471079799</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="2">_xlfn.CHISQ.INV(1-$D$1,A3)</f>
+        <v>10.596634733096071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>6.2513886311703235</v>
+        <v>11.344866730144364</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
         <v>7.8147279032511774</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>12.838156466598644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>7.779440339734859</v>
+        <v>13.276704135987615</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
         <v>9.4877290367811575</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>14.860259000560278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>9.2363568997811178</v>
+        <v>15.086272469388986</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
         <v>11.070497693516351</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>16.749602343639047</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>10.64464067566842</v>
+        <v>16.811893829770934</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
         <v>12.591587243743977</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>18.547584178511098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>12.017036623780532</v>
+        <v>18.475306906582354</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
         <v>14.067140449340165</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>20.277739874962634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>13.361566136511726</v>
+        <v>20.090235029663219</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
         <v>15.507313055865449</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>21.954954990659523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>14.683656573259837</v>
+        <v>21.66599433346191</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
         <v>16.918977604620448</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>23.589350781257416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>15.987179172105261</v>
+        <v>23.209251158954348</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
         <v>18.307038053275139</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>25.188179571971148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>17.275008517500076</v>
+        <v>24.724970311318277</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
         <v>19.675137572682495</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>26.756848916469661</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>18.549347786703244</v>
+        <v>26.216967305535864</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
         <v>21.026069817483062</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>28.299518822046032</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>19.811929307127564</v>
+        <v>27.688249610457024</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
         <v>22.362032494826938</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>29.819471223653263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>21.064144212997061</v>
+        <v>29.141237740672786</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
         <v>23.684791304840573</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>31.319349622595272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>22.307129581578693</v>
+        <v>30.577914166892491</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
         <v>24.995790139728623</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>32.801320645791876</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>23.541828923096112</v>
+        <v>31.999926908815176</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
         <v>26.296227604864239</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>34.267186537826703</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>24.769035343901454</v>
+        <v>33.408663605004612</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
         <v>27.587111638275317</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>35.718465659004622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>25.989423082637213</v>
+        <v>34.805305734705065</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
         <v>28.869299430392626</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>37.156451456606774</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>27.203571029356826</v>
+        <v>36.190869129270048</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
         <v>30.143527205646159</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>38.58225655493419</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>28.411980584305631</v>
+        <v>37.566234786625039</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
         <v>31.410432844230925</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>39.996846312938665</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>29.615089436182725</v>
+        <v>38.932172683516065</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
         <v>32.670573340917301</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>41.401064771417637</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>30.813282343953034</v>
+        <v>40.289360437593885</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
         <v>33.924438471443807</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>42.795654999308503</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>32.006899681704304</v>
+        <v>41.638398118858461</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
         <v>35.172461626908046</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>44.181275249971065</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>33.196244288628179</v>
+        <v>42.979820139351617</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
         <v>36.415028501807313</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>45.558511936530564</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>34.381587017552953</v>
+        <v>44.314104896219163</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
         <v>37.652484133482773</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>46.927890160080736</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>35.563171271923466</v>
+        <v>45.641682666283138</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
         <v>38.885138659830041</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>48.289882332456827</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>36.741216747797644</v>
+        <v>46.962942124751436</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
         <v>40.113272069413618</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>49.644915298994228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>37.915922544697068</v>
+        <v>48.278235770315511</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
         <v>41.337138151427389</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>50.99337626849946</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>39.087469770693957</v>
+        <v>49.587884472898864</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
         <v>42.556967804292675</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>52.335617785933636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>40.256023738711804</v>
+        <v>50.892181311517106</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
         <v>43.772971825742189</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>53.671961930240641</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>41.42173582978522</v>
+        <v>52.1913948331919</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
         <v>44.985343280365136</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>55.002703880023894</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>42.584745082980838</v>
+        <v>53.48577183623533</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
         <v>46.194259520278464</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>56.328114959710852</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>43.745179559434199</v>
+        <v>54.775539760110348</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
         <v>47.399883919080914</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>57.64844525585854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>44.903157518519933</v>
+        <v>56.060908747789085</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
         <v>48.602367367294185</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>58.963925875519337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>46.058788436836693</v>
+        <v>57.342073433859248</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
         <v>49.801849568201852</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>60.274770904781029</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>47.212173894937365</v>
+        <v>58.619214501687068</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
         <v>50.998460165710647</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>61.581179114757276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>48.363408352194348</v>
+        <v>59.892500045086891</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
         <v>52.192319730102867</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>62.883335453741203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>49.512579826575553</v>
+        <v>61.162086763689679</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
         <v>53.383540622969299</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>64.181412357406231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>50.65977049321372</v>
+        <v>62.428121016184875</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
         <v>54.572227758941722</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>65.475570903468039</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>51.805057213317518</v>
+        <v>63.690739751564493</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
         <v>55.75847927888703</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>66.765961832803967</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>52.94851200308203</v>
+        <v>64.950071335211192</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
         <v>56.942387146824096</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>68.052726455441544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>54.090202450712404</v>
+        <v>66.206236283993249</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
         <v>58.124037680868021</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>69.335997456900387</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>55.230192088408906</v>
+        <v>67.459347922325819</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
         <v>59.303512026899803</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>70.615899617966335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>56.368540725118756</v>
+        <v>68.709512969345425</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
         <v>60.480886582336446</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>71.89255045899921</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>57.505304744995996</v>
+        <v>69.956832065838213</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
         <v>61.656233376279566</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>73.166060818225091</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>58.640537375791716</v>
+        <v>71.201400248311543</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
         <v>62.829620411408186</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>74.436535372101758</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>59.774288930795954</v>
+        <v>72.443307376548233</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
         <v>64.001111972218027</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>75.704073104694814</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>60.906607027448374</v>
+        <v>73.682638520105741</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
         <v>65.170768903569837</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>76.96876773204454</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>62.037536785309669</v>
+        <v>74.919474308478186</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
         <v>66.33864886296881</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>78.230708086689958</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>63.167121005726322</v>
+        <v>76.153891249012702</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
         <v>67.504806549541186</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>79.489978466828958</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>64.295400335215845</v>
+        <v>77.385962016137285</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
         <v>68.669293912285795</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>80.746658954013284</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>65.422413414339772</v>
+        <v>78.615755715002479</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
         <v>69.832160339848116</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>82.00082570277533</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>66.548197013609254</v>
+        <v>79.843338122251453</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
         <v>70.993452833782271</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>83.252551205161083</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>67.672786157777495</v>
+        <v>81.068771906297115</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
         <v>72.153216167023089</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>84.50190453277645</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>68.796214239709329</v>
+        <v>82.292116829199642</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
         <v>73.311493029083252</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>85.748951558640982</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>69.91851312487637</v>
+        <v>83.513429931989407</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
         <v>74.468324159309361</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>86.993755160871714</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>71.039713247404336</v>
+        <v>84.732765705063827</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
         <v>75.623748469376054</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>88.236375409982116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>72.159843698492153</v>
+        <v>85.950176245103449</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
         <v>76.777803156061481</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>89.476869741381122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>73.27893230793083</v>
+        <v>87.165711399787568</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
         <v>77.930523805230422</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>90.71529311447577</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>74.397005719368593</v>
+        <v>88.379418901449341</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
         <v>79.08194448784873</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>91.951698159629785</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>75.514089459899182</v>
+        <v>89.591344490687078</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
         <v>80.23209784876272</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>93.186135314089086</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>76.630208004487741</v>
+        <v>90.801532030838715</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
         <v>81.381015188899099</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>94.418652947874449</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>77.745384835694892</v>
+        <v>92.010023614131995</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
         <v>82.528726541471798</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>95.649297480528389</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>78.859642499111601</v>
+        <v>93.216859660238427</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
         <v>83.67526074272098</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>96.878113489517872</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>79.973002654875458</v>
+        <v>94.422079007885074</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
         <v>84.82064549765667</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>98.105143811009455</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B130" si="2">_xlfn.CHISQ.INV(1-$B$1,A67)</f>
-        <v>81.085486125601648</v>
+        <f t="shared" ref="B67:B130" si="3">_xlfn.CHISQ.INV(1-$B$1,A67)</f>
+        <v>95.625719000112895</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="3">_xlfn.CHISQ.INV(1-$C$1,A67)</f>
+        <f t="shared" ref="C67:C130" si="4">_xlfn.CHISQ.INV(1-$C$1,A67)</f>
         <v>85.964907441230963</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="5">_xlfn.CHISQ.INV(1-$D$1,A67)</f>
+        <v>99.330429633663201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
-        <f t="shared" si="2"/>
-        <v>82.19711294102899</v>
+        <f t="shared" si="3"/>
+        <v>96.827815563712306</v>
       </c>
       <c r="C68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.10807219532191</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>100.55401058602804</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" si="2"/>
-        <v>83.307902379651907</v>
+        <f t="shared" si="3"/>
+        <v>98.028403283314077</v>
       </c>
       <c r="C69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88.250164421874118</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>101.77592481806394</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" si="2"/>
-        <v>84.417873007583594</v>
+        <f t="shared" si="3"/>
+        <v>99.227515470569443</v>
       </c>
       <c r="C70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.391207872507962</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>102.99620907726474</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" si="2"/>
-        <v>85.527042714871882</v>
+        <f t="shared" si="3"/>
+        <v>100.42518422881135</v>
       </c>
       <c r="C71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.531225434880653</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>104.21489877981668</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" si="2"/>
-        <v>86.635428749469213</v>
+        <f t="shared" si="3"/>
+        <v>101.62144051355199</v>
       </c>
       <c r="C72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.670239176054849</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>105.43202807717712</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" si="2"/>
-        <v>87.743047749039036</v>
+        <f t="shared" si="3"/>
+        <v>102.81631418914067</v>
       </c>
       <c r="C73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92.808270383107711</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <f t="shared" si="5"/>
+        <v>106.64762991843352</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" si="2"/>
-        <v>88.849915770764937</v>
+        <f t="shared" si="3"/>
+        <v>104.00983408187497</v>
       </c>
       <c r="C74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93.945339601192245</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <f t="shared" si="5"/>
+        <v>107.86173610876281</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" si="2"/>
-        <v>89.956048319313538</v>
+        <f t="shared" si="3"/>
+        <v>105.20202802983309</v>
       </c>
       <c r="C75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.081466669243241</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <f t="shared" si="5"/>
+        <v>109.07437736428484</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" si="2"/>
-        <v>91.061460373088977</v>
+        <f t="shared" si="3"/>
+        <v>106.39292292967178</v>
       </c>
       <c r="C76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96.216670753503834</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <f t="shared" si="5"/>
+        <v>110.28558336357985</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" si="2"/>
-        <v>92.166166408904999</v>
+        <f t="shared" si="3"/>
+        <v>107.58254478061225</v>
       </c>
       <c r="C77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.350970379032958</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <f t="shared" si="5"/>
+        <v>111.49538279611278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" si="2"/>
-        <v>93.270180425189608</v>
+        <f t="shared" si="3"/>
+        <v>108.77091872581829</v>
       </c>
       <c r="C78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.484383459340421</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <f t="shared" si="5"/>
+        <v>112.70380340778992</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" si="2"/>
-        <v>94.373515963827373</v>
+        <f t="shared" si="3"/>
+        <v>109.95806909135278</v>
       </c>
       <c r="C79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99.616927324283836</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <f t="shared" si="5"/>
+        <v>113.91087204385181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" si="2"/>
-        <v>95.476186130736224</v>
+        <f t="shared" si="3"/>
+        <v>111.14401942288374</v>
       </c>
       <c r="C80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100.74861874635032</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <f t="shared" si="5"/>
+        <v>115.11661468929169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="2"/>
-        <v>96.578203615267014</v>
+        <f t="shared" si="3"/>
+        <v>112.3287925202973</v>
       </c>
       <c r="C81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101.87947396543588</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>116.32105650696919</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
-        <f t="shared" si="2"/>
-        <v>97.679580708507032</v>
+        <f t="shared" si="3"/>
+        <v>113.51241047036054</v>
       </c>
       <c r="C82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103.00950871222616</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>117.52422187358148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
-        <f t="shared" si="2"/>
-        <v>98.780329320562501</v>
+        <f t="shared" si="3"/>
+        <v>114.69489467756806</v>
       </c>
       <c r="C83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104.13873823027387</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>118.72613441363418</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84">
-        <f t="shared" si="2"/>
-        <v>99.88046099688853</v>
+        <f t="shared" si="3"/>
+        <v>115.87626589329336</v>
       </c>
       <c r="C84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>105.26717729686032</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>119.92681703154784</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
-        <f t="shared" si="2"/>
-        <v>100.9799869337301</v>
+        <f t="shared" si="3"/>
+        <v>117.05654424335819</v>
       </c>
       <c r="C85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106.39484024272251</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>121.12629194202354</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
-        <f t="shared" si="2"/>
-        <v>102.0789179927325</v>
+        <f t="shared" si="3"/>
+        <v>118.23574925412316</v>
       </c>
       <c r="C86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>107.52174097071945</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>122.32458069878128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
-        <f t="shared" si="2"/>
-        <v>103.17726471477495</v>
+        <f t="shared" si="3"/>
+        <v>119.41389987719508</v>
       </c>
       <c r="C87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108.64789297350761</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>123.52170422177649</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
-        <f t="shared" si="2"/>
-        <v>104.27503733307771</v>
+        <f t="shared" si="3"/>
+        <v>120.59101451284056</v>
       </c>
       <c r="C88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109.77330935028795</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>124.71768282299236</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
-        <f t="shared" si="2"/>
-        <v>105.37224578562838</v>
+        <f t="shared" si="3"/>
+        <v>121.76711103218737</v>
       </c>
       <c r="C89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110.89800282268448</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>125.91253623089737</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
-        <f t="shared" si="2"/>
-        <v>106.46889972697032</v>
+        <f t="shared" si="3"/>
+        <v>122.94220679828861</v>
       </c>
       <c r="C90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>112.02198574980785</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>127.10628361365266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
-        <f t="shared" si="2"/>
-        <v>107.56500853939279</v>
+        <f t="shared" si="3"/>
+        <v>124.1163186861213</v>
       </c>
       <c r="C91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>113.1452701425554</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>128.29894360114542</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
-        <f t="shared" si="2"/>
-        <v>108.66058134355924</v>
+        <f t="shared" si="3"/>
+        <v>125.28946310158366</v>
       </c>
       <c r="C92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>114.26786767719354</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>129.49053430592045</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
-        <f t="shared" si="2"/>
-        <v>109.75562700860829</v>
+        <f t="shared" si="3"/>
+        <v>126.46165599955258</v>
       </c>
       <c r="C93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115.38978970826685</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>130.68107334307626</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
-        <f t="shared" si="2"/>
-        <v>110.85015416175854</v>
+        <f t="shared" si="3"/>
+        <v>127.63291290105587</v>
       </c>
       <c r="C94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>116.51104728087354</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>131.87057784918849</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95">
-        <f t="shared" si="2"/>
-        <v>111.94417119744713</v>
+        <f t="shared" si="3"/>
+        <v>128.80324890961415</v>
       </c>
       <c r="C95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>117.63165114234553</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>133.05906450031728</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96">
-        <f t="shared" si="2"/>
-        <v>113.037686286029</v>
+        <f t="shared" si="3"/>
+        <v>129.97267872679876</v>
       </c>
       <c r="C96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>118.75161175336736</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>134.24654952915242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97">
-        <f t="shared" si="2"/>
-        <v>114.13070738206275</v>
+        <f t="shared" si="3"/>
+        <v>131.14121666705202</v>
       </c>
       <c r="C97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119.87093929856714</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>135.43304874134594</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98">
-        <f t="shared" si="2"/>
-        <v>115.22324223220659</v>
+        <f t="shared" si="3"/>
+        <v>132.30887667181258</v>
       </c>
       <c r="C98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120.98964369660956</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>136.61857753108038</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
-        <f t="shared" si="2"/>
-        <v>116.31529838274675</v>
+        <f t="shared" si="3"/>
+        <v>133.47567232298491</v>
       </c>
       <c r="C99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122.10773460981942</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>137.80315089591301</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100">
-        <f t="shared" si="2"/>
-        <v>117.4068831867789</v>
+        <f t="shared" si="3"/>
+        <v>134.6416168557891</v>
       </c>
       <c r="C100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>123.2252214533618</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>138.98678345093953</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101">
-        <f t="shared" si="2"/>
-        <v>118.49800381106211</v>
+        <f t="shared" si="3"/>
+        <v>135.80672317102679</v>
       </c>
       <c r="C101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124.34211340400408</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>140.16948944231359</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102">
-        <f t="shared" si="2"/>
-        <v>119.58866724256319</v>
+        <f t="shared" si="3"/>
+        <v>136.97100384679408</v>
       </c>
       <c r="C102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125.45841940848237</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <f t="shared" si="5"/>
+        <v>141.35128276015851</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103">
-        <f t="shared" si="2"/>
-        <v>120.67888029470862</v>
+        <f t="shared" si="3"/>
+        <v>138.13447114967266</v>
       </c>
       <c r="C103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126.57414819149434</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <f t="shared" si="5"/>
+        <v>142.53217695090208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104">
-        <f t="shared" si="2"/>
-        <v>121.76864961335946</v>
+        <f t="shared" si="3"/>
+        <v>139.29713704542647</v>
       </c>
       <c r="C104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127.68930826333825</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <f t="shared" si="5"/>
+        <v>143.71218522906958</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105">
-        <f t="shared" si="2"/>
-        <v>122.85798168252468</v>
+        <f t="shared" si="3"/>
+        <v>140.45901320923065</v>
       </c>
       <c r="C105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128.80390792721764</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>144.8913204885589</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106">
-        <f t="shared" si="2"/>
-        <v>123.94688282982615</v>
+        <f t="shared" si="3"/>
+        <v>141.62011103545771</v>
       </c>
       <c r="C106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129.91795528622893</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>146.06959531343026</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107">
-        <f t="shared" si="2"/>
-        <v>125.03535923172883</v>
+        <f t="shared" si="3"/>
+        <v>142.7804416470438</v>
       </c>
       <c r="C107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131.03145825004873</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>147.24702198823161</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108">
-        <f t="shared" si="2"/>
-        <v>126.12341691854816</v>
+        <f t="shared" si="3"/>
+        <v>143.94001590445714</v>
       </c>
       <c r="C108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>132.14442454133663</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>148.42361250788713</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109">
-        <f t="shared" si="2"/>
-        <v>127.21106177924611</v>
+        <f t="shared" si="3"/>
+        <v>145.09884441428903</v>
       </c>
       <c r="C109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>133.25686170186819</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>149.59937858716816</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110">
-        <f t="shared" si="2"/>
-        <v>128.29829956602683</v>
+        <f t="shared" si="3"/>
+        <v>146.25693753748627</v>
       </c>
       <c r="C110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>134.36877709841121</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <f t="shared" si="5"/>
+        <v>150.77433166977215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111">
-        <f t="shared" si="2"/>
-        <v>129.38513589874199</v>
+        <f t="shared" si="3"/>
+        <v>147.41430539724425</v>
       </c>
       <c r="C111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>135.4801779283595</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111">
+        <f t="shared" si="5"/>
+        <v>151.94848293702353</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112">
-        <f t="shared" si="2"/>
-        <v>130.47157626911522</v>
+        <f t="shared" si="3"/>
+        <v>148.57095788657577</v>
       </c>
       <c r="C112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136.59107122513501</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112">
+        <f t="shared" si="5"/>
+        <v>153.12184331622157</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113">
-        <f t="shared" si="2"/>
-        <v>131.55762604479483</v>
+        <f t="shared" si="3"/>
+        <v>149.72690467557402</v>
       </c>
       <c r="C113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>137.70146386337072</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113">
+        <f t="shared" si="5"/>
+        <v>154.29442348864833</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114">
-        <f t="shared" si="2"/>
-        <v>132.64329047324318</v>
+        <f t="shared" si="3"/>
+        <v>150.88215521838262</v>
       </c>
       <c r="C114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138.8113625638847</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114">
+        <f t="shared" si="5"/>
+        <v>155.4662338972542</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115">
-        <f t="shared" si="2"/>
-        <v>133.72857468547085</v>
+        <f t="shared" si="3"/>
+        <v>152.03671875988823</v>
       </c>
       <c r="C115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>139.92077389845574</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115">
+        <f t="shared" si="5"/>
+        <v>156.63728475404</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116">
-        <f t="shared" si="2"/>
-        <v>134.81348369962248</v>
+        <f t="shared" si="3"/>
+        <v>153.19060434214893</v>
       </c>
       <c r="C116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>141.02970429440973</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>157.80758604714447</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117">
-        <f t="shared" si="2"/>
-        <v>135.89802242442258</v>
+        <f t="shared" si="3"/>
+        <v>154.34382081057055</v>
       </c>
       <c r="C117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>142.13816003902647</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117">
+        <f t="shared" si="5"/>
+        <v>158.97714754765715</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118">
-        <f t="shared" si="2"/>
-        <v>136.98219566248659</v>
+        <f t="shared" si="3"/>
+        <v>155.4963768198437</v>
       </c>
       <c r="C118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>143.24614728377486</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118">
+        <f t="shared" si="5"/>
+        <v>160.14597881616493</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119">
-        <f t="shared" si="2"/>
-        <v>138.06600811350464</v>
+        <f t="shared" si="3"/>
+        <v>156.64828083965185</v>
       </c>
       <c r="C119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>144.35367204838508</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119">
+        <f t="shared" si="5"/>
+        <v>161.31408920904838</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120">
-        <f t="shared" si="2"/>
-        <v>139.14946437730339</v>
+        <f t="shared" si="3"/>
+        <v>157.79954116016174</v>
       </c>
       <c r="C120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>145.46074022476483</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120">
+        <f t="shared" si="5"/>
+        <v>162.4814878845375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121">
-        <f t="shared" si="2"/>
-        <v>140.23256895679179</v>
+        <f t="shared" si="3"/>
+        <v>158.95016589730628</v>
       </c>
       <c r="C121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>146.56735758076746</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121">
+        <f t="shared" si="5"/>
+        <v>163.64818380853754</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
       <c r="B122">
-        <f t="shared" si="2"/>
-        <v>141.31532626079596</v>
+        <f t="shared" si="3"/>
+        <v>160.10016299786872</v>
       </c>
       <c r="C122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>147.67352976381807</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122">
+        <f t="shared" si="5"/>
+        <v>164.81418576023793</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123">
-        <f t="shared" si="2"/>
-        <v>142.39774060678846</v>
+        <f t="shared" si="3"/>
+        <v>161.24954024437844</v>
       </c>
       <c r="C123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>148.77926230440488</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123">
+        <f t="shared" si="5"/>
+        <v>165.97950233751141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124">
-        <f t="shared" si="2"/>
-        <v>143.47981622351656</v>
+        <f t="shared" si="3"/>
+        <v>162.39830525982492</v>
       </c>
       <c r="C124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>149.88456061944134</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D124">
+        <f t="shared" si="5"/>
+        <v>167.14414196211465</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
       <c r="B125">
-        <f t="shared" si="2"/>
-        <v>144.56155725353412</v>
+        <f t="shared" si="3"/>
+        <v>163.54646551219997</v>
       </c>
       <c r="C125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150.98943001550484</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D125">
+        <f t="shared" si="5"/>
+        <v>168.30811288469889</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
       <c r="B126">
-        <f t="shared" si="2"/>
-        <v>145.64296775564111</v>
+        <f t="shared" si="3"/>
+        <v>164.69402831887504</v>
       </c>
       <c r="C126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>152.09387569195783</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D126">
+        <f t="shared" si="5"/>
+        <v>169.47142318963759</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
       <c r="B127">
-        <f t="shared" si="2"/>
-        <v>146.72405170723547</v>
+        <f t="shared" si="3"/>
+        <v>165.84100085082048</v>
       </c>
       <c r="C127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>153.19790274395621</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D127">
+        <f t="shared" si="5"/>
+        <v>170.6340807996817</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
       <c r="B128">
-        <f t="shared" si="2"/>
-        <v>147.80481300658039</v>
+        <f t="shared" si="3"/>
+        <v>166.98739013667389</v>
       </c>
       <c r="C128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>154.30151616535022</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D128">
+        <f t="shared" si="5"/>
+        <v>171.79609348044747</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129">
-        <f t="shared" si="2"/>
-        <v>148.88525547499117</v>
+        <f t="shared" si="3"/>
+        <v>168.13320306666489</v>
       </c>
       <c r="C129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>155.40472085148204</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D129">
+        <f t="shared" si="5"/>
+        <v>172.9574688447465</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130">
-        <f t="shared" si="2"/>
-        <v>149.96538285894493</v>
+        <f t="shared" si="3"/>
+        <v>169.27844639640136</v>
       </c>
       <c r="C130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156.50752160188514</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D130">
+        <f t="shared" si="5"/>
+        <v>174.11821435676239</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
       <c r="B131">
-        <f t="shared" ref="B131:B140" si="4">_xlfn.CHISQ.INV(1-$B$1,A131)</f>
-        <v>151.04519883211674</v>
+        <f t="shared" ref="B131:B140" si="6">_xlfn.CHISQ.INV(1-$B$1,A131)</f>
+        <v>170.42312675052347</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C140" si="5">_xlfn.CHISQ.INV(1-$C$1,A131)</f>
+        <f t="shared" ref="C131:C140" si="7">_xlfn.CHISQ.INV(1-$C$1,A131)</f>
         <v>157.60992312288906</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131">
+        <f t="shared" ref="D131:D140" si="8">_xlfn.CHISQ.INV(1-$D$1,A131)</f>
+        <v>175.27833733608259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
       <c r="B132">
-        <f t="shared" si="4"/>
-        <v>152.1247069973447</v>
+        <f t="shared" si="6"/>
+        <v>171.56725062623141</v>
       </c>
       <c r="C132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>158.71193003013371</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D132">
+        <f t="shared" si="8"/>
+        <v>176.43784496159012</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
       <c r="B133">
-        <f t="shared" si="4"/>
-        <v>153.20391088852773</v>
+        <f t="shared" si="6"/>
+        <v>172.71082439669203</v>
       </c>
       <c r="C133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>159.8135468509978</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133">
+        <f t="shared" si="8"/>
+        <v>177.59674427522222</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
       <c r="B134">
-        <f t="shared" si="4"/>
-        <v>154.28281397245826</v>
+        <f t="shared" si="6"/>
+        <v>173.85385431432846</v>
       </c>
       <c r="C134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>160.91477802694322</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D134">
+        <f t="shared" si="8"/>
+        <v>178.75504218559999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
       <c r="B135">
-        <f t="shared" si="4"/>
-        <v>155.36141965059272</v>
+        <f t="shared" si="6"/>
+        <v>174.99634651399933</v>
       </c>
       <c r="C135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>162.01562791578101</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D135">
+        <f t="shared" si="8"/>
+        <v>179.91274547153625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136">
-        <f t="shared" si="4"/>
-        <v>156.4397312607627</v>
+        <f t="shared" si="6"/>
+        <v>176.13830701607091</v>
       </c>
       <c r="C136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>163.11610079386037</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D136">
+        <f t="shared" si="8"/>
+        <v>181.06986078542502</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
       <c r="B137">
-        <f t="shared" si="4"/>
-        <v>157.51775207882852</v>
+        <f t="shared" si="6"/>
+        <v>177.2797417293863</v>
       </c>
       <c r="C137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>164.21620085818489</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D137">
+        <f t="shared" si="8"/>
+        <v>182.22639465651773</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
       <c r="B138">
-        <f t="shared" si="4"/>
-        <v>158.5954853202783</v>
+        <f t="shared" si="6"/>
+        <v>178.42065645413678</v>
       </c>
       <c r="C138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>165.31593222845851</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D138">
+        <f t="shared" si="8"/>
+        <v>183.38235349409246</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
       <c r="B139">
-        <f t="shared" si="4"/>
-        <v>159.67293414177416</v>
+        <f t="shared" si="6"/>
+        <v>179.56105688463896</v>
       </c>
       <c r="C139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>166.41529894906409</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D139">
+        <f t="shared" si="8"/>
+        <v>184.53774359051724</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
       <c r="B140">
-        <f t="shared" si="4"/>
-        <v>160.75010164264802</v>
+        <f t="shared" si="6"/>
+        <v>180.7009486120208</v>
       </c>
       <c r="C140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>167.51430499097765</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="8"/>
+        <v>185.69257112421434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>